<commit_message>
update the analys user file (The convert file to json )
</commit_message>
<xml_diff>
--- a/analyse_user_data/user_places_list.xlsx
+++ b/analyse_user_data/user_places_list.xlsx
@@ -6,15 +6,18 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Data" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Places</t>
+    <t>"- The Gourmet Bistro</t>
+  </si>
+  <si>
+    <t>Sunshine Café"</t>
   </si>
 </sst>
 </file>
@@ -59,7 +62,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -70,6 +73,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>